<commit_message>
custom functions using chatgpt in lab apps removed
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_scenario_en.xlsx
+++ b/sample_apps/lab_app_en/lab_app_scenario_en.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FC75AA-88B4-491D-AACC-E7C8E18A47A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D372D514-3BBE-4D18-A1B4-A297E6D71F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="75">
   <si>
     <t>conditions</t>
     <phoneticPr fontId="1"/>
@@ -254,18 +254,10 @@
     <t>confirmed-if-have-sandwich</t>
   </si>
   <si>
-    <t>{impression} . Thank you for your time.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#final_with_impression</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>set_impression_of_dialogue(&amp;impression)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>#final_abort</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -323,6 +315,9 @@
   </si>
   <si>
     <t>$"Please determine if the user said the reason."</t>
+  </si>
+  <si>
+    <t>{$"Generate a short utterance to say the system's impression."} Thank you for your time.</t>
   </si>
 </sst>
 </file>
@@ -775,24 +770,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" style="6"/>
+    <col min="1" max="1" width="8.5703125" style="6"/>
     <col min="2" max="2" width="28" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.86328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.59765625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="40.265625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="46.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.59765625" style="6"/>
+    <col min="3" max="3" width="36.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -832,7 +827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="28.5">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -840,13 +835,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>45</v>
@@ -863,7 +858,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="42.75">
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="45">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -871,7 +866,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -900,7 +895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="28.5">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -911,13 +906,13 @@
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" ht="42.75">
+    <row r="8" spans="1:8" s="10" customFormat="1" ht="45">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -954,7 +949,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="28.5">
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="45">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -965,7 +960,7 @@
         <v>36</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>54</v>
@@ -983,7 +978,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="F11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
@@ -1000,7 +995,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="7" t="s">
@@ -1024,7 +1019,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>11</v>
@@ -1044,7 +1039,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="7" customFormat="1" ht="28.5">
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1052,13 +1047,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>22</v>
@@ -1072,10 +1067,10 @@
         <v>8</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" s="8" customFormat="1" ht="28.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
@@ -1092,16 +1087,16 @@
         <v>16</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H17" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="8" customFormat="1" ht="28.5">
+    <row r="18" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
@@ -1118,13 +1113,13 @@
         <v>37</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H18" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="8" customFormat="1" ht="28.5">
+    <row r="19" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="42.75">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="45">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1154,14 +1149,11 @@
       <c r="C20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="H20" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="28.5">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1174,14 +1166,11 @@
       <c r="D21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>58</v>
-      </c>
       <c r="H21" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" ht="28.5">
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1194,14 +1183,11 @@
       <c r="D22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="H22" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" ht="57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="9" customFormat="1" ht="60">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
@@ -1209,40 +1195,40 @@
         <v>22</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" ht="28.5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="9" customFormat="1" ht="30">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A25" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="30">
+      <c r="A26" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="28.5">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="C26" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1">

</xml_diff>

<commit_message>
chatgpt ner block finished
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_scenario_en.xlsx
+++ b/sample_apps/lab_app_en/lab_app_scenario_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3FC75AA-88B4-491D-AACC-E7C8E18A47A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD6EB52-2BA3-4BE6-8871-C1E70B157FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
+    <workbookView xWindow="6975" yWindow="2820" windowWidth="21600" windowHeight="11055" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
   <sheets>
     <sheet name="scenario" sheetId="1" r:id="rId1"/>
@@ -294,13 +294,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>#NE_PERSON!=""</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Thank you {#NE_PERSON}! Let me ask you about sandwich. Do you have sandwiches very often?</t>
-  </si>
-  <si>
     <t>{greeting}. I'm {get_system_name()}. If you don't mind, could you tell me your name?</t>
   </si>
   <si>
@@ -323,6 +316,12 @@
   </si>
   <si>
     <t>$"Please determine if the user said the reason."</t>
+  </si>
+  <si>
+    <t>Thank you {#NE_person}! Let me ask you about sandwich. Do you have sandwiches very often?</t>
+  </si>
+  <si>
+    <t>#NE_person!=""</t>
   </si>
 </sst>
 </file>
@@ -775,24 +774,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.59765625" style="6"/>
+    <col min="1" max="1" width="8.5703125" style="6"/>
     <col min="2" max="2" width="28" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.86328125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.59765625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="40.265625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="46.3984375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.59765625" style="6"/>
+    <col min="3" max="3" width="36.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.5703125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -832,7 +831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="5" customFormat="1" ht="28.5">
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -840,13 +839,13 @@
         <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>45</v>
@@ -863,7 +862,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" ht="42.75">
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="45">
       <c r="A5" s="3" t="s">
         <v>20</v>
       </c>
@@ -871,7 +870,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -900,7 +899,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="28.5">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
@@ -911,13 +910,13 @@
         <v>36</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="10" customFormat="1" ht="42.75">
+    <row r="8" spans="1:8" s="10" customFormat="1" ht="45">
       <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
@@ -954,7 +953,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" ht="28.5">
+    <row r="10" spans="1:8" s="10" customFormat="1" ht="45">
       <c r="A10" s="10" t="s">
         <v>20</v>
       </c>
@@ -965,7 +964,7 @@
         <v>36</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>54</v>
@@ -1024,7 +1023,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>11</v>
@@ -1044,7 +1043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="7" customFormat="1" ht="28.5">
+    <row r="15" spans="1:8" s="7" customFormat="1" ht="30">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1052,13 +1051,13 @@
         <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>22</v>
@@ -1075,7 +1074,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="8" customFormat="1" ht="28.5">
+    <row r="17" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A17" s="8" t="s">
         <v>20</v>
       </c>
@@ -1092,7 +1091,7 @@
         <v>16</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>63</v>
@@ -1101,7 +1100,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="8" customFormat="1" ht="28.5">
+    <row r="18" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
@@ -1124,7 +1123,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="8" customFormat="1" ht="28.5">
+    <row r="19" spans="1:8" s="8" customFormat="1" ht="30">
       <c r="A19" s="8" t="s">
         <v>20</v>
       </c>
@@ -1144,7 +1143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="4" customFormat="1" ht="42.75">
+    <row r="20" spans="1:8" s="4" customFormat="1" ht="45">
       <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="28.5">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="45">
       <c r="A21" s="5" t="s">
         <v>20</v>
       </c>
@@ -1181,7 +1180,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="3" customFormat="1" ht="28.5">
+    <row r="22" spans="1:8" s="3" customFormat="1" ht="30">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1201,7 +1200,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="9" customFormat="1" ht="57">
+    <row r="23" spans="1:8" s="9" customFormat="1" ht="60">
       <c r="A23" s="9" t="s">
         <v>20</v>
       </c>
@@ -1209,10 +1208,10 @@
         <v>22</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="9" customFormat="1" ht="28.5">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="9" customFormat="1" ht="30">
       <c r="A24" s="9" t="s">
         <v>20</v>
       </c>
@@ -1234,7 +1233,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="28.5">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="30">
       <c r="A26" s="5" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
system instruction allowed, some bugs fixed
</commit_message>
<xml_diff>
--- a/sample_apps/lab_app_en/lab_app_scenario_en.xlsx
+++ b/sample_apps/lab_app_en/lab_app_scenario_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nakano\system\dialbb\dialbb-next\sample_apps\lab_app_en\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC3C1FB-A955-40E6-949B-32B1E5B2DC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346DD122-E29B-4676-B0BB-9EBD0996A2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C3566FB2-A815-41D8-9347-99D11DD601B4}"/>
   </bookViews>
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9D1DC6-E066-4D71-9ECD-01107058A46B}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15"/>
@@ -997,7 +997,7 @@
         <v>63</v>
       </c>
       <c r="G12" s="3"/>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>